<commit_message>
S2R und R2S Packete hinzugefügt
</commit_message>
<xml_diff>
--- a/FucktionalPoints.xlsx
+++ b/FucktionalPoints.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\SWEngineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\310113053\Documents\software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5010" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5010" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="73">
   <si>
     <t>Einstufung</t>
   </si>
@@ -209,6 +209,48 @@
   </si>
   <si>
     <t>Score S2R</t>
+  </si>
+  <si>
+    <t>H2 ist vorhanden</t>
+  </si>
+  <si>
+    <t>Berechnung ist erfolgreich</t>
+  </si>
+  <si>
+    <t>Prüfer will Bewertung ausrechnen</t>
+  </si>
+  <si>
+    <t>1. Prüfer muss H2 Bewertung einstellen</t>
+  </si>
+  <si>
+    <t>2. Das Programm berechnet eine Rate</t>
+  </si>
+  <si>
+    <t>3. Rate wird abgespeichert</t>
+  </si>
+  <si>
+    <t>Weitere Parameters / Impacts (R2S) können folgen</t>
+  </si>
+  <si>
+    <t>Score R2S</t>
+  </si>
+  <si>
+    <t>S2R ist vorhanden</t>
+  </si>
+  <si>
+    <t>Weitere Parameters / Impacts sollen in den Score eingerechnet werden</t>
+  </si>
+  <si>
+    <t>Prüfer will weitere Parameters einbinden</t>
+  </si>
+  <si>
+    <t>1. Prüfer muss S2R besitzen</t>
+  </si>
+  <si>
+    <t>2. Das Programm berechnet weite Parameters / Impacts</t>
+  </si>
+  <si>
+    <t>3. Neue Rate wird abgespeichert</t>
   </si>
 </sst>
 </file>
@@ -248,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,7 +574,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -638,7 +680,7 @@
       <selection activeCell="B12" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
@@ -744,7 +786,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.28515625" bestFit="1" customWidth="1"/>
@@ -850,7 +892,7 @@
       <selection activeCell="B12" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.28515625" bestFit="1" customWidth="1"/>
@@ -956,7 +998,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.28515625" bestFit="1" customWidth="1"/>
@@ -1057,7 +1099,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
@@ -1159,11 +1201,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
@@ -1187,7 +1229,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1195,7 +1237,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1261,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1227,17 +1269,17 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1245,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1253,7 +1295,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1265,11 +1307,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
@@ -1277,7 +1319,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1293,7 +1335,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1301,7 +1343,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1325,7 +1367,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1333,17 +1375,17 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1359,7 +1401,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1373,7 +1415,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>